<commit_message>
updated default costs spreadsheet
</commit_message>
<xml_diff>
--- a/References/Wind Default Costs.xlsx
+++ b/References/Wind Default Costs.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23730" windowHeight="15330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Proposed 2016.3.14" sheetId="3" r:id="rId1"/>
+    <sheet name="2014.11.24" sheetId="2" r:id="rId2"/>
+    <sheet name="2014.1.14" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -19,6 +21,160 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>NREL</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>NREL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+http://energy.gov/sites/prod/files/2015/08/f25/2014-Distributed-Wind-Market-Report-8.7_0.pdf</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>NREL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+http://www.nrel.gov/docs/fy16osti/64281.pdf 2014 COE Review Table ES1. Don't include financial costs because those numbers are handled in SAM's financial models!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>NREL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+http://www.nrel.gov/docs/fy16osti/64281.pdf Table ES2. Don't include financing costs because those are handled in SAM's financial models!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>NREL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This was incorrectly including financing costs previously</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>NREL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+No way currently to include it in defaults, but have it as reference just in case</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>NREL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Percentage calculated using Table 2 in 2013 Distributed Wind Market Report where turbine = turbine + tower to be consistent with utility-scale. This table was not recreated in 2014 Distributed wind Market Report</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>NREL</author>
@@ -102,7 +258,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
   <si>
     <t>Fixed Annual Cost ($/yr)</t>
   </si>
@@ -219,13 +375,110 @@
   </si>
   <si>
     <t>Proposed -2012 Report</t>
+  </si>
+  <si>
+    <t>Utility</t>
+  </si>
+  <si>
+    <t>Onshore</t>
+  </si>
+  <si>
+    <t>Offshore</t>
+  </si>
+  <si>
+    <t>Turbine Cost ($/kW)</t>
+  </si>
+  <si>
+    <t>BOS Cost ($/kW)</t>
+  </si>
+  <si>
+    <t>Total Cost ($/kW)</t>
+  </si>
+  <si>
+    <t>O&amp;M Cost ($/MWh)</t>
+  </si>
+  <si>
+    <t>Res/Comm</t>
+  </si>
+  <si>
+    <t>Proposed</t>
+  </si>
+  <si>
+    <t>Existing</t>
+  </si>
+  <si>
+    <t>http://www.nrel.gov/docs/fy16osti/64281.pdf</t>
+  </si>
+  <si>
+    <t>Table ES1</t>
+  </si>
+  <si>
+    <t>Table ES2</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>http://energy.gov/sites/prod/files/2015/08/f25/2014-Distributed-Wind-Market-Report-8.7_0.pdf</t>
+  </si>
+  <si>
+    <t>Exec Summary</t>
+  </si>
+  <si>
+    <t>Distributed (Res/Comm) Total Cost</t>
+  </si>
+  <si>
+    <t>** 10-120 $/kW</t>
+  </si>
+  <si>
+    <t>Utility-Scale Onshore Costs*</t>
+  </si>
+  <si>
+    <t>Utility-Scale Offshore Costs*</t>
+  </si>
+  <si>
+    <t>*"Market price adjustors" in the table are ignored per Chris Mone and Tyler Stehly 3/7/16</t>
+  </si>
+  <si>
+    <t>this is because in the paper they are assumed to be applied to financing costs.</t>
+  </si>
+  <si>
+    <t>Residential Breakdown:</t>
+  </si>
+  <si>
+    <t>to be consistent with utility-scale</t>
+  </si>
+  <si>
+    <t>Turbine = turbine + tower in Table 2</t>
+  </si>
+  <si>
+    <t>BOS = everything else in Table 2</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>Turbine/Total (%)</t>
+  </si>
+  <si>
+    <t>Blue= calculated</t>
+  </si>
+  <si>
+    <t>Distributed (Res/Comm) Percentage of Turbine/Total</t>
+  </si>
+  <si>
+    <t>http://www.energy.gov/sites/prod/files/2014/09/f18/2013%20Distributed%20Wind%20Market%20Report.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,8 +515,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,6 +584,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -298,10 +606,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -319,18 +630,43 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="8" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="8" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="8" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -345,6 +681,49 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>466058</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>142619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4962525" y="381000"/>
+          <a:ext cx="5342858" cy="2047619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -356,34 +735,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -600,7 +979,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -608,10 +987,377 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="16" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="17" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="32">
+        <v>6230</v>
+      </c>
+      <c r="C4" s="24">
+        <v>6940</v>
+      </c>
+      <c r="D4" s="28">
+        <f>D5+D6</f>
+        <v>1566</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29">
+        <f>F5+F6</f>
+        <v>4229</v>
+      </c>
+      <c r="G4" s="29">
+        <f>G5+G6</f>
+        <v>5187</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="27">
+        <f>B4*B8</f>
+        <v>4194.5956448419975</v>
+      </c>
+      <c r="C5" s="24">
+        <v>4673</v>
+      </c>
+      <c r="D5" s="23">
+        <v>1221</v>
+      </c>
+      <c r="E5" s="23">
+        <v>1029</v>
+      </c>
+      <c r="F5" s="23">
+        <v>1952</v>
+      </c>
+      <c r="G5" s="23">
+        <v>1660</v>
+      </c>
+      <c r="J5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="27">
+        <f>(1-B8)*B4</f>
+        <v>2035.4043551580025</v>
+      </c>
+      <c r="C6" s="24">
+        <v>2267</v>
+      </c>
+      <c r="D6" s="23">
+        <v>345</v>
+      </c>
+      <c r="E6" s="25">
+        <v>601</v>
+      </c>
+      <c r="F6" s="23">
+        <v>2277</v>
+      </c>
+      <c r="G6" s="23">
+        <v>3527</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="22">
+        <v>9</v>
+      </c>
+      <c r="D7" s="23">
+        <v>15</v>
+      </c>
+      <c r="E7" s="23">
+        <v>9</v>
+      </c>
+      <c r="F7" s="31">
+        <v>39</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="36">
+        <f>(14145+31770)/68195</f>
+        <v>0.67328983063274439</v>
+      </c>
+      <c r="C8" s="37">
+        <v>0.67</v>
+      </c>
+      <c r="D8" s="35">
+        <f>D5/D4</f>
+        <v>0.77969348659003834</v>
+      </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="34">
+        <f>F5/F4</f>
+        <v>0.46157484038779856</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="J8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="24">
+        <v>6940</v>
+      </c>
+      <c r="C3" s="23">
+        <v>1630</v>
+      </c>
+      <c r="D3" s="23">
+        <v>5187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="24">
+        <v>4673</v>
+      </c>
+      <c r="C4" s="23">
+        <v>1029</v>
+      </c>
+      <c r="D4" s="23">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="24">
+        <v>2267</v>
+      </c>
+      <c r="C5" s="23">
+        <v>601</v>
+      </c>
+      <c r="D5" s="23">
+        <v>3527</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="22">
+        <v>9</v>
+      </c>
+      <c r="C6" s="21">
+        <v>9</v>
+      </c>
+      <c r="D6" s="21">
+        <v>9</v>
+      </c>
+      <c r="O6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,10 +1389,10 @@
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="14"/>
       <c r="D3" s="7" t="s">
         <v>23</v>
       </c>
@@ -743,19 +1489,19 @@
       <c r="F9" s="6">
         <v>90</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
     </row>
     <row r="10" spans="1:17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1071,7 +1817,7 @@
       <c r="B28" s="1">
         <v>2600</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D28" s="6">
@@ -1119,31 +1865,31 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="11">
         <v>2540</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="11">
         <v>2810</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33" s="11">
         <v>6960</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="13" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated all wind default costs
</commit_message>
<xml_diff>
--- a/References/Wind Default Costs.xlsx
+++ b/References/Wind Default Costs.xlsx
@@ -258,7 +258,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
   <si>
     <t>Fixed Annual Cost ($/yr)</t>
   </si>
@@ -468,6 +468,9 @@
   </si>
   <si>
     <t>http://www.energy.gov/sites/prod/files/2014/09/f18/2013%20Distributed%20Wind%20Market%20Report.pdf</t>
+  </si>
+  <si>
+    <t>**Commercial uses residential Turbine/BOS costs and utility O&amp;M costs</t>
   </si>
 </sst>
 </file>
@@ -476,7 +479,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -633,12 +636,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -646,21 +643,27 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="8" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="9" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="9" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="8" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -979,7 +982,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -987,119 +990,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="16" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="17" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="17"/>
+    <col min="2" max="2" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="14" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="15" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="19"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="17" t="s">
         <v>48</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B4" s="30">
         <v>6230</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="22">
         <v>6940</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="26">
         <f>D5+D6</f>
         <v>1566</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29">
+      <c r="E4" s="27"/>
+      <c r="F4" s="27">
         <f>F5+F6</f>
         <v>4229</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="27">
         <f>G5+G6</f>
         <v>5187</v>
       </c>
-      <c r="J4" s="33" t="s">
+      <c r="J4" s="31" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="25">
         <f>B4*B8</f>
         <v>4194.5956448419975</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="22">
         <v>4673</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="21">
         <v>1221</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="21">
         <v>1029</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="21">
         <v>1952</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="21">
         <v>1660</v>
       </c>
       <c r="J5" t="s">
@@ -1107,26 +1110,26 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="25">
         <f>(1-B8)*B4</f>
         <v>2035.4043551580025</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="22">
         <v>2267</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="21">
         <v>345</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="23">
         <v>601</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="21">
         <v>2277</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="21">
         <v>3527</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -1137,22 +1140,22 @@
       <c r="A7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="21">
+        <v>15</v>
+      </c>
+      <c r="E7" s="21">
         <v>9</v>
       </c>
-      <c r="D7" s="23">
-        <v>15</v>
-      </c>
-      <c r="E7" s="23">
-        <v>9</v>
-      </c>
-      <c r="F7" s="31">
+      <c r="F7" s="29">
         <v>39</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="19" t="s">
         <v>52</v>
       </c>
       <c r="J7" t="s">
@@ -1163,29 +1166,29 @@
       <c r="A8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="36">
+      <c r="B8" s="34">
         <f>(14145+31770)/68195</f>
         <v>0.67328983063274439</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="35">
         <v>0.67</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="33">
         <f>D5/D4</f>
         <v>0.77969348659003834</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="34">
+      <c r="E8" s="21"/>
+      <c r="F8" s="32">
         <f>F5/F4</f>
         <v>0.46157484038779856</v>
       </c>
-      <c r="G8" s="21"/>
+      <c r="G8" s="19"/>
       <c r="J8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="14" t="s">
         <v>56</v>
       </c>
       <c r="J9" s="2" t="s">
@@ -1198,7 +1201,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="28" t="s">
         <v>67</v>
       </c>
       <c r="J11" t="s">
@@ -1223,6 +1226,11 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1246,28 +1254,28 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="17"/>
+    <col min="2" max="2" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="19"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="17" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1275,41 +1283,41 @@
       <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="22">
         <v>6940</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="21">
         <v>1630</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="21">
         <v>5187</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="22">
         <v>4673</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="21">
         <v>1029</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="21">
         <v>1660</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="22">
         <v>2267</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="21">
         <v>601</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="21">
         <v>3527</v>
       </c>
     </row>
@@ -1317,13 +1325,13 @@
       <c r="A6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="20">
         <v>9</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="19">
         <v>9</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="19">
         <v>9</v>
       </c>
       <c r="O6" t="s">
@@ -1389,10 +1397,10 @@
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="14"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="7" t="s">
         <v>23</v>
       </c>
@@ -1489,19 +1497,19 @@
       <c r="F9" s="6">
         <v>90</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
     </row>
     <row r="10" spans="1:17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">

</xml_diff>